<commit_message>
version estable 20230214 1540
</commit_message>
<xml_diff>
--- a/backup/lectura 52 semanas.doc.xlsx
+++ b/backup/lectura 52 semanas.doc.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\0 - A Repositorios GitHub\Devocionales\backup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22110" windowHeight="9555" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="587">
   <si>
     <t>Semana</t>
   </si>
@@ -1768,12 +1773,24 @@
   </si>
   <si>
     <t>Tito &amp; Filemón</t>
+  </si>
+  <si>
+    <t>Levítico (1 a 2)</t>
+  </si>
+  <si>
+    <t>Levítico (2 a 4)</t>
+  </si>
+  <si>
+    <t>Levítico (5 a 9)</t>
+  </si>
+  <si>
+    <t>Levítico (10 a 14)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1783,12 +1800,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1803,8 +1826,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1814,6 +1838,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1862,7 +1889,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1897,7 +1924,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2113,15 +2140,15 @@
       <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2147,7 +2174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2173,7 +2200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>73</v>
       </c>
@@ -2196,7 +2223,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2222,7 +2249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>80</v>
       </c>
@@ -2245,7 +2272,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2271,7 +2298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>87</v>
       </c>
@@ -2294,7 +2321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2320,7 +2347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>94</v>
       </c>
@@ -2343,7 +2370,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2369,7 +2396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>89</v>
       </c>
@@ -2392,7 +2419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -2418,7 +2445,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -2441,7 +2468,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2467,7 +2494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>101</v>
       </c>
@@ -2490,7 +2517,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -2516,7 +2543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>83</v>
       </c>
@@ -2539,7 +2566,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2565,7 +2592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>78</v>
       </c>
@@ -2588,7 +2615,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -2614,7 +2641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>91</v>
       </c>
@@ -2637,7 +2664,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -2663,7 +2690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>122</v>
       </c>
@@ -2686,7 +2713,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -2712,7 +2739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -2735,7 +2762,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13</v>
       </c>
@@ -2761,7 +2788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>127</v>
       </c>
@@ -2784,7 +2811,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
@@ -2810,7 +2837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>123</v>
       </c>
@@ -2833,7 +2860,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15</v>
       </c>
@@ -2859,7 +2886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>135</v>
       </c>
@@ -2882,7 +2909,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>16</v>
       </c>
@@ -2908,7 +2935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>121</v>
       </c>
@@ -2931,7 +2958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>17</v>
       </c>
@@ -2957,7 +2984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -2980,7 +3007,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>18</v>
       </c>
@@ -3006,7 +3033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>94</v>
       </c>
@@ -3029,7 +3056,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>19</v>
       </c>
@@ -3055,7 +3082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>76</v>
       </c>
@@ -3078,7 +3105,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20</v>
       </c>
@@ -3104,7 +3131,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>144</v>
       </c>
@@ -3127,7 +3154,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>21</v>
       </c>
@@ -3153,7 +3180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>92</v>
       </c>
@@ -3176,7 +3203,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>22</v>
       </c>
@@ -3202,7 +3229,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>149</v>
       </c>
@@ -3225,7 +3252,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>23</v>
       </c>
@@ -3251,7 +3278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>154</v>
       </c>
@@ -3274,7 +3301,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>24</v>
       </c>
@@ -3300,7 +3327,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>158</v>
       </c>
@@ -3323,7 +3350,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>25</v>
       </c>
@@ -3349,7 +3376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>165</v>
       </c>
@@ -3372,7 +3399,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>26</v>
       </c>
@@ -3398,7 +3425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>172</v>
       </c>
@@ -3421,7 +3448,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>27</v>
       </c>
@@ -3447,7 +3474,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>177</v>
       </c>
@@ -3470,7 +3497,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>28</v>
       </c>
@@ -3496,7 +3523,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>80</v>
       </c>
@@ -3519,7 +3546,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>29</v>
       </c>
@@ -3545,7 +3572,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>73</v>
       </c>
@@ -3568,7 +3595,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>30</v>
       </c>
@@ -3594,7 +3621,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>80</v>
       </c>
@@ -3617,7 +3644,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>31</v>
       </c>
@@ -3643,7 +3670,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>188</v>
       </c>
@@ -3666,7 +3693,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>32</v>
       </c>
@@ -3692,7 +3719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>73</v>
       </c>
@@ -3715,7 +3742,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>33</v>
       </c>
@@ -3741,7 +3768,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>194</v>
       </c>
@@ -3764,7 +3791,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>34</v>
       </c>
@@ -3790,7 +3817,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>196</v>
       </c>
@@ -3813,7 +3840,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>35</v>
       </c>
@@ -3839,7 +3866,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>89</v>
       </c>
@@ -3862,7 +3889,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>36</v>
       </c>
@@ -3888,7 +3915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>110</v>
       </c>
@@ -3911,7 +3938,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>37</v>
       </c>
@@ -3937,7 +3964,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>86</v>
       </c>
@@ -3960,7 +3987,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>38</v>
       </c>
@@ -3986,7 +4013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>89</v>
       </c>
@@ -4009,7 +4036,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>39</v>
       </c>
@@ -4035,7 +4062,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>89</v>
       </c>
@@ -4055,7 +4082,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>40</v>
       </c>
@@ -4081,7 +4108,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>204</v>
       </c>
@@ -4104,7 +4131,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>41</v>
       </c>
@@ -4130,7 +4157,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>136</v>
       </c>
@@ -4153,7 +4180,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>42</v>
       </c>
@@ -4179,7 +4206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>201</v>
       </c>
@@ -4202,7 +4229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>43</v>
       </c>
@@ -4228,7 +4255,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>208</v>
       </c>
@@ -4251,7 +4278,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>44</v>
       </c>
@@ -4277,7 +4304,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>210</v>
       </c>
@@ -4300,7 +4327,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>45</v>
       </c>
@@ -4326,7 +4353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>135</v>
       </c>
@@ -4349,7 +4376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>46</v>
       </c>
@@ -4375,7 +4402,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>105</v>
       </c>
@@ -4398,7 +4425,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>47</v>
       </c>
@@ -4424,7 +4451,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>78</v>
       </c>
@@ -4447,7 +4474,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>48</v>
       </c>
@@ -4473,7 +4500,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>89</v>
       </c>
@@ -4496,7 +4523,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>49</v>
       </c>
@@ -4522,7 +4549,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>92</v>
       </c>
@@ -4545,7 +4572,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>50</v>
       </c>
@@ -4571,7 +4598,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>73</v>
       </c>
@@ -4594,7 +4621,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>51</v>
       </c>
@@ -4620,7 +4647,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>90</v>
       </c>
@@ -4643,7 +4670,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>52</v>
       </c>
@@ -4669,7 +4696,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>70</v>
       </c>
@@ -4703,15 +4730,17 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4737,7 +4766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4763,7 +4792,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4789,7 +4818,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4815,7 +4844,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4841,7 +4870,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4867,7 +4896,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4893,7 +4922,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4919,7 +4948,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4945,7 +4974,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4971,7 +5000,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4997,7 +5026,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5023,7 +5052,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5049,7 +5078,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5075,7 +5104,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5101,7 +5130,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5127,7 +5156,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5153,7 +5182,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5179,7 +5208,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5205,7 +5234,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5231,7 +5260,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5257,7 +5286,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5283,7 +5312,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5309,7 +5338,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5335,7 +5364,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5361,7 +5390,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5387,7 +5416,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5413,7 +5442,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5439,7 +5468,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5465,7 +5494,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5491,7 +5520,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5517,7 +5546,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5543,7 +5572,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5569,7 +5598,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5595,7 +5624,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5621,7 +5650,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5647,7 +5676,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5673,7 +5702,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5699,7 +5728,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5725,7 +5754,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5751,7 +5780,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5777,7 +5806,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5803,7 +5832,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5829,7 +5858,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5855,7 +5884,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5881,7 +5910,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5907,7 +5936,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5933,7 +5962,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5959,7 +5988,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5985,7 +6014,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6011,7 +6040,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6037,7 +6066,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6063,7 +6092,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6097,12 +6126,1397 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C6" t="s">
+        <v>584</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="E6" t="s">
+        <v>586</v>
+      </c>
+      <c r="F6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G6" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" t="s">
+        <v>264</v>
+      </c>
+      <c r="F8" t="s">
+        <v>265</v>
+      </c>
+      <c r="G8" t="s">
+        <v>266</v>
+      </c>
+      <c r="H8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F9" t="s">
+        <v>272</v>
+      </c>
+      <c r="G9" t="s">
+        <v>273</v>
+      </c>
+      <c r="H9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" t="s">
+        <v>277</v>
+      </c>
+      <c r="E10" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" t="s">
+        <v>279</v>
+      </c>
+      <c r="G10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E11" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" t="s">
+        <v>286</v>
+      </c>
+      <c r="G11" t="s">
+        <v>287</v>
+      </c>
+      <c r="H11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" t="s">
+        <v>291</v>
+      </c>
+      <c r="E12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F12" t="s">
+        <v>293</v>
+      </c>
+      <c r="G12" t="s">
+        <v>294</v>
+      </c>
+      <c r="H12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" t="s">
+        <v>300</v>
+      </c>
+      <c r="G13" t="s">
+        <v>301</v>
+      </c>
+      <c r="H13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" t="s">
+        <v>304</v>
+      </c>
+      <c r="D14" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" t="s">
+        <v>306</v>
+      </c>
+      <c r="F14" t="s">
+        <v>307</v>
+      </c>
+      <c r="G14" t="s">
+        <v>308</v>
+      </c>
+      <c r="H14" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
+        <v>312</v>
+      </c>
+      <c r="E15" t="s">
+        <v>313</v>
+      </c>
+      <c r="F15" t="s">
+        <v>314</v>
+      </c>
+      <c r="G15" t="s">
+        <v>315</v>
+      </c>
+      <c r="H15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>317</v>
+      </c>
+      <c r="C16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D16" t="s">
+        <v>319</v>
+      </c>
+      <c r="E16" t="s">
+        <v>320</v>
+      </c>
+      <c r="F16" t="s">
+        <v>321</v>
+      </c>
+      <c r="G16" t="s">
+        <v>322</v>
+      </c>
+      <c r="H16" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>324</v>
+      </c>
+      <c r="C17" t="s">
+        <v>325</v>
+      </c>
+      <c r="D17" t="s">
+        <v>326</v>
+      </c>
+      <c r="E17" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17" t="s">
+        <v>328</v>
+      </c>
+      <c r="G17" t="s">
+        <v>329</v>
+      </c>
+      <c r="H17" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C18" t="s">
+        <v>332</v>
+      </c>
+      <c r="D18" t="s">
+        <v>333</v>
+      </c>
+      <c r="E18" t="s">
+        <v>334</v>
+      </c>
+      <c r="F18" t="s">
+        <v>335</v>
+      </c>
+      <c r="G18" t="s">
+        <v>336</v>
+      </c>
+      <c r="H18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>338</v>
+      </c>
+      <c r="C19" t="s">
+        <v>339</v>
+      </c>
+      <c r="D19" t="s">
+        <v>340</v>
+      </c>
+      <c r="E19" t="s">
+        <v>341</v>
+      </c>
+      <c r="F19" t="s">
+        <v>342</v>
+      </c>
+      <c r="G19" t="s">
+        <v>343</v>
+      </c>
+      <c r="H19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>345</v>
+      </c>
+      <c r="C20" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" t="s">
+        <v>347</v>
+      </c>
+      <c r="E20" t="s">
+        <v>348</v>
+      </c>
+      <c r="F20" t="s">
+        <v>349</v>
+      </c>
+      <c r="G20" t="s">
+        <v>350</v>
+      </c>
+      <c r="H20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>352</v>
+      </c>
+      <c r="C21" t="s">
+        <v>353</v>
+      </c>
+      <c r="D21" t="s">
+        <v>354</v>
+      </c>
+      <c r="E21" t="s">
+        <v>355</v>
+      </c>
+      <c r="F21" t="s">
+        <v>356</v>
+      </c>
+      <c r="G21" t="s">
+        <v>357</v>
+      </c>
+      <c r="H21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>359</v>
+      </c>
+      <c r="C22" t="s">
+        <v>360</v>
+      </c>
+      <c r="D22" t="s">
+        <v>361</v>
+      </c>
+      <c r="E22" t="s">
+        <v>362</v>
+      </c>
+      <c r="F22" t="s">
+        <v>363</v>
+      </c>
+      <c r="G22" t="s">
+        <v>364</v>
+      </c>
+      <c r="H22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>366</v>
+      </c>
+      <c r="C23" t="s">
+        <v>367</v>
+      </c>
+      <c r="D23" t="s">
+        <v>368</v>
+      </c>
+      <c r="E23" t="s">
+        <v>369</v>
+      </c>
+      <c r="F23" t="s">
+        <v>370</v>
+      </c>
+      <c r="G23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>373</v>
+      </c>
+      <c r="C24" t="s">
+        <v>374</v>
+      </c>
+      <c r="D24" t="s">
+        <v>375</v>
+      </c>
+      <c r="E24" t="s">
+        <v>376</v>
+      </c>
+      <c r="F24" t="s">
+        <v>377</v>
+      </c>
+      <c r="G24" t="s">
+        <v>378</v>
+      </c>
+      <c r="H24" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>380</v>
+      </c>
+      <c r="C25" t="s">
+        <v>381</v>
+      </c>
+      <c r="D25" t="s">
+        <v>382</v>
+      </c>
+      <c r="E25" t="s">
+        <v>383</v>
+      </c>
+      <c r="F25" t="s">
+        <v>384</v>
+      </c>
+      <c r="G25" t="s">
+        <v>385</v>
+      </c>
+      <c r="H25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C26" t="s">
+        <v>388</v>
+      </c>
+      <c r="D26" t="s">
+        <v>389</v>
+      </c>
+      <c r="E26" t="s">
+        <v>390</v>
+      </c>
+      <c r="F26" t="s">
+        <v>391</v>
+      </c>
+      <c r="G26" t="s">
+        <v>392</v>
+      </c>
+      <c r="H26" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>394</v>
+      </c>
+      <c r="C27" t="s">
+        <v>395</v>
+      </c>
+      <c r="D27" t="s">
+        <v>396</v>
+      </c>
+      <c r="E27" t="s">
+        <v>397</v>
+      </c>
+      <c r="F27" t="s">
+        <v>398</v>
+      </c>
+      <c r="G27" t="s">
+        <v>399</v>
+      </c>
+      <c r="H27" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>401</v>
+      </c>
+      <c r="C28" t="s">
+        <v>402</v>
+      </c>
+      <c r="D28" t="s">
+        <v>403</v>
+      </c>
+      <c r="E28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F28" t="s">
+        <v>405</v>
+      </c>
+      <c r="G28" t="s">
+        <v>406</v>
+      </c>
+      <c r="H28" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>408</v>
+      </c>
+      <c r="C29" t="s">
+        <v>409</v>
+      </c>
+      <c r="D29" t="s">
+        <v>410</v>
+      </c>
+      <c r="E29" t="s">
+        <v>411</v>
+      </c>
+      <c r="F29" t="s">
+        <v>412</v>
+      </c>
+      <c r="G29" t="s">
+        <v>413</v>
+      </c>
+      <c r="H29" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>415</v>
+      </c>
+      <c r="C30" t="s">
+        <v>416</v>
+      </c>
+      <c r="D30" t="s">
+        <v>417</v>
+      </c>
+      <c r="E30" t="s">
+        <v>418</v>
+      </c>
+      <c r="F30" t="s">
+        <v>419</v>
+      </c>
+      <c r="G30" t="s">
+        <v>420</v>
+      </c>
+      <c r="H30" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>422</v>
+      </c>
+      <c r="C31" t="s">
+        <v>423</v>
+      </c>
+      <c r="D31" t="s">
+        <v>424</v>
+      </c>
+      <c r="E31" t="s">
+        <v>425</v>
+      </c>
+      <c r="F31" t="s">
+        <v>426</v>
+      </c>
+      <c r="G31" t="s">
+        <v>427</v>
+      </c>
+      <c r="H31" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>429</v>
+      </c>
+      <c r="C32" t="s">
+        <v>430</v>
+      </c>
+      <c r="D32" t="s">
+        <v>431</v>
+      </c>
+      <c r="E32" t="s">
+        <v>432</v>
+      </c>
+      <c r="F32" t="s">
+        <v>433</v>
+      </c>
+      <c r="G32" t="s">
+        <v>434</v>
+      </c>
+      <c r="H32" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>436</v>
+      </c>
+      <c r="C33" t="s">
+        <v>437</v>
+      </c>
+      <c r="D33" t="s">
+        <v>438</v>
+      </c>
+      <c r="E33" t="s">
+        <v>439</v>
+      </c>
+      <c r="F33" t="s">
+        <v>440</v>
+      </c>
+      <c r="G33" t="s">
+        <v>441</v>
+      </c>
+      <c r="H33" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>443</v>
+      </c>
+      <c r="C34" t="s">
+        <v>444</v>
+      </c>
+      <c r="D34" t="s">
+        <v>445</v>
+      </c>
+      <c r="E34" t="s">
+        <v>446</v>
+      </c>
+      <c r="F34" t="s">
+        <v>447</v>
+      </c>
+      <c r="G34" t="s">
+        <v>448</v>
+      </c>
+      <c r="H34" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>450</v>
+      </c>
+      <c r="C35" t="s">
+        <v>451</v>
+      </c>
+      <c r="D35" t="s">
+        <v>452</v>
+      </c>
+      <c r="E35" t="s">
+        <v>453</v>
+      </c>
+      <c r="F35" t="s">
+        <v>454</v>
+      </c>
+      <c r="G35" t="s">
+        <v>455</v>
+      </c>
+      <c r="H35" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>457</v>
+      </c>
+      <c r="C36" t="s">
+        <v>458</v>
+      </c>
+      <c r="D36" t="s">
+        <v>459</v>
+      </c>
+      <c r="E36" t="s">
+        <v>460</v>
+      </c>
+      <c r="F36" t="s">
+        <v>461</v>
+      </c>
+      <c r="G36" t="s">
+        <v>462</v>
+      </c>
+      <c r="H36" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>464</v>
+      </c>
+      <c r="C37" t="s">
+        <v>465</v>
+      </c>
+      <c r="D37" t="s">
+        <v>466</v>
+      </c>
+      <c r="E37" t="s">
+        <v>467</v>
+      </c>
+      <c r="F37" t="s">
+        <v>468</v>
+      </c>
+      <c r="G37" t="s">
+        <v>469</v>
+      </c>
+      <c r="H37" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>471</v>
+      </c>
+      <c r="C38" t="s">
+        <v>472</v>
+      </c>
+      <c r="D38" t="s">
+        <v>473</v>
+      </c>
+      <c r="E38" t="s">
+        <v>474</v>
+      </c>
+      <c r="F38" t="s">
+        <v>475</v>
+      </c>
+      <c r="G38" t="s">
+        <v>476</v>
+      </c>
+      <c r="H38" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>478</v>
+      </c>
+      <c r="C39" t="s">
+        <v>479</v>
+      </c>
+      <c r="D39" t="s">
+        <v>480</v>
+      </c>
+      <c r="E39" t="s">
+        <v>481</v>
+      </c>
+      <c r="F39" t="s">
+        <v>482</v>
+      </c>
+      <c r="G39" t="s">
+        <v>483</v>
+      </c>
+      <c r="H39" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>485</v>
+      </c>
+      <c r="C40" t="s">
+        <v>486</v>
+      </c>
+      <c r="D40" t="s">
+        <v>487</v>
+      </c>
+      <c r="E40" t="s">
+        <v>488</v>
+      </c>
+      <c r="F40" t="s">
+        <v>489</v>
+      </c>
+      <c r="G40" t="s">
+        <v>490</v>
+      </c>
+      <c r="H40" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>492</v>
+      </c>
+      <c r="C41" t="s">
+        <v>493</v>
+      </c>
+      <c r="D41" t="s">
+        <v>494</v>
+      </c>
+      <c r="E41" t="s">
+        <v>495</v>
+      </c>
+      <c r="F41" t="s">
+        <v>496</v>
+      </c>
+      <c r="G41" t="s">
+        <v>497</v>
+      </c>
+      <c r="H41" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>499</v>
+      </c>
+      <c r="C42" t="s">
+        <v>500</v>
+      </c>
+      <c r="D42" t="s">
+        <v>501</v>
+      </c>
+      <c r="E42" t="s">
+        <v>502</v>
+      </c>
+      <c r="F42" t="s">
+        <v>503</v>
+      </c>
+      <c r="G42" t="s">
+        <v>504</v>
+      </c>
+      <c r="H42" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>506</v>
+      </c>
+      <c r="C43" t="s">
+        <v>507</v>
+      </c>
+      <c r="D43" t="s">
+        <v>508</v>
+      </c>
+      <c r="E43" t="s">
+        <v>509</v>
+      </c>
+      <c r="F43" t="s">
+        <v>510</v>
+      </c>
+      <c r="G43" t="s">
+        <v>511</v>
+      </c>
+      <c r="H43" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>513</v>
+      </c>
+      <c r="C44" t="s">
+        <v>514</v>
+      </c>
+      <c r="D44" t="s">
+        <v>515</v>
+      </c>
+      <c r="E44" t="s">
+        <v>516</v>
+      </c>
+      <c r="F44" t="s">
+        <v>517</v>
+      </c>
+      <c r="G44" t="s">
+        <v>518</v>
+      </c>
+      <c r="H44" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>520</v>
+      </c>
+      <c r="C45" t="s">
+        <v>521</v>
+      </c>
+      <c r="D45" t="s">
+        <v>522</v>
+      </c>
+      <c r="E45" t="s">
+        <v>523</v>
+      </c>
+      <c r="F45" t="s">
+        <v>524</v>
+      </c>
+      <c r="G45" t="s">
+        <v>525</v>
+      </c>
+      <c r="H45" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>527</v>
+      </c>
+      <c r="C46" t="s">
+        <v>528</v>
+      </c>
+      <c r="D46" t="s">
+        <v>529</v>
+      </c>
+      <c r="E46" t="s">
+        <v>530</v>
+      </c>
+      <c r="F46" t="s">
+        <v>531</v>
+      </c>
+      <c r="G46" t="s">
+        <v>532</v>
+      </c>
+      <c r="H46" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>534</v>
+      </c>
+      <c r="C47" t="s">
+        <v>535</v>
+      </c>
+      <c r="D47" t="s">
+        <v>536</v>
+      </c>
+      <c r="E47" t="s">
+        <v>537</v>
+      </c>
+      <c r="F47" t="s">
+        <v>538</v>
+      </c>
+      <c r="G47" t="s">
+        <v>539</v>
+      </c>
+      <c r="H47" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>541</v>
+      </c>
+      <c r="C48" t="s">
+        <v>542</v>
+      </c>
+      <c r="D48" t="s">
+        <v>543</v>
+      </c>
+      <c r="E48" t="s">
+        <v>544</v>
+      </c>
+      <c r="F48" t="s">
+        <v>545</v>
+      </c>
+      <c r="G48" t="s">
+        <v>546</v>
+      </c>
+      <c r="H48" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>548</v>
+      </c>
+      <c r="C49" t="s">
+        <v>549</v>
+      </c>
+      <c r="D49" t="s">
+        <v>550</v>
+      </c>
+      <c r="E49" t="s">
+        <v>551</v>
+      </c>
+      <c r="F49" t="s">
+        <v>552</v>
+      </c>
+      <c r="G49" t="s">
+        <v>553</v>
+      </c>
+      <c r="H49" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>555</v>
+      </c>
+      <c r="C50" t="s">
+        <v>556</v>
+      </c>
+      <c r="D50" t="s">
+        <v>557</v>
+      </c>
+      <c r="E50" t="s">
+        <v>558</v>
+      </c>
+      <c r="F50" t="s">
+        <v>559</v>
+      </c>
+      <c r="G50" t="s">
+        <v>560</v>
+      </c>
+      <c r="H50" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>562</v>
+      </c>
+      <c r="C51" t="s">
+        <v>563</v>
+      </c>
+      <c r="D51" t="s">
+        <v>564</v>
+      </c>
+      <c r="E51" t="s">
+        <v>565</v>
+      </c>
+      <c r="F51" t="s">
+        <v>566</v>
+      </c>
+      <c r="G51" t="s">
+        <v>582</v>
+      </c>
+      <c r="H51" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>568</v>
+      </c>
+      <c r="C52" t="s">
+        <v>569</v>
+      </c>
+      <c r="D52" t="s">
+        <v>570</v>
+      </c>
+      <c r="E52" t="s">
+        <v>571</v>
+      </c>
+      <c r="F52" t="s">
+        <v>572</v>
+      </c>
+      <c r="G52" t="s">
+        <v>573</v>
+      </c>
+      <c r="H52" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>581</v>
+      </c>
+      <c r="C53" t="s">
+        <v>575</v>
+      </c>
+      <c r="D53" t="s">
+        <v>576</v>
+      </c>
+      <c r="E53" t="s">
+        <v>577</v>
+      </c>
+      <c r="F53" t="s">
+        <v>578</v>
+      </c>
+      <c r="G53" t="s">
+        <v>579</v>
+      </c>
+      <c r="H53" t="s">
+        <v>580</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
version estable 20230214 2126
</commit_message>
<xml_diff>
--- a/backup/lectura 52 semanas.doc.xlsx
+++ b/backup/lectura 52 semanas.doc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="589">
   <si>
     <t>Semana</t>
   </si>
@@ -1785,6 +1785,12 @@
   </si>
   <si>
     <t>Levítico (10 a 14)</t>
+  </si>
+  <si>
+    <t>Sabado</t>
+  </si>
+  <si>
+    <t>Miercoles</t>
   </si>
 </sst>
 </file>
@@ -6129,7 +6135,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6149,7 +6155,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>588</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -6158,7 +6164,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>587</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Version Estable 20230215 092341
</commit_message>
<xml_diff>
--- a/backup/lectura 52 semanas.doc.xlsx
+++ b/backup/lectura 52 semanas.doc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\0 - A Repositorios GitHub\Devocionales\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector Martinez\Documents\0 - A Repositorios GitHub\Devocionales\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22110" windowHeight="9555" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1796,7 +1796,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2146,15 +2146,15 @@
       <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>73</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>80</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>87</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>94</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>89</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>101</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>83</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>78</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>91</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>122</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>13</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>127</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>14</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>123</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>15</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>135</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>16</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>121</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>17</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>18</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>94</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>19</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>76</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>144</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>21</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>92</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>22</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>149</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>23</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>154</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>24</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>158</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>25</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>165</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>26</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>172</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>27</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>177</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>28</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>80</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>29</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>73</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>30</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>80</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>31</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>188</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>32</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>73</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>33</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>194</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>34</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>196</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>35</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>89</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>36</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>110</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>37</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>86</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>38</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>89</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>39</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>89</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>40</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>204</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>41</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>136</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>42</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>201</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>43</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>208</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>44</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>210</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>45</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>135</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>46</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>105</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>47</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>78</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>48</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>89</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>49</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>92</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>50</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>73</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>51</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>90</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>52</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>70</v>
       </c>
@@ -4740,13 +4740,13 @@
       <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6135,16 +6135,16 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6664,7 +6664,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
version estable 20230215 1358
</commit_message>
<xml_diff>
--- a/backup/lectura 52 semanas.doc.xlsx
+++ b/backup/lectura 52 semanas.doc.xlsx
@@ -9,22 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$H$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hoja4!$A$3:$I$107</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="593">
   <si>
     <t>Semana</t>
   </si>
@@ -1791,13 +1794,28 @@
   </si>
   <si>
     <t>Miercoles</t>
+  </si>
+  <si>
+    <t>Plan de Lectura Biblico - 52 Semanas</t>
+  </si>
+  <si>
+    <t>Pasaje</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>desg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1805,8 +1823,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1819,8 +1871,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1828,15 +1896,189 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6134,8 +6376,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection sqref="A1:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7525,4 +7767,4306 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja4"/>
+  <dimension ref="A1:I135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="20.44140625" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="B1" s="46"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45" t="s">
+        <v>589</v>
+      </c>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="35">
+        <v>1</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="40">
+        <v>1</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>591</v>
+      </c>
+      <c r="C5" s="20">
+        <v>44942</v>
+      </c>
+      <c r="D5" s="21">
+        <v>44943</v>
+      </c>
+      <c r="E5" s="21">
+        <v>44944</v>
+      </c>
+      <c r="F5" s="21">
+        <v>44945</v>
+      </c>
+      <c r="G5" s="21">
+        <v>44946</v>
+      </c>
+      <c r="H5" s="21">
+        <v>44947</v>
+      </c>
+      <c r="I5" s="22">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="35">
+        <v>2</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="42">
+        <v>2</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C7" s="20">
+        <v>44949</v>
+      </c>
+      <c r="D7" s="21">
+        <v>44950</v>
+      </c>
+      <c r="E7" s="21">
+        <v>44951</v>
+      </c>
+      <c r="F7" s="21">
+        <v>44952</v>
+      </c>
+      <c r="G7" s="21">
+        <v>44953</v>
+      </c>
+      <c r="H7" s="21">
+        <v>44954</v>
+      </c>
+      <c r="I7" s="22">
+        <v>44955</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="35">
+        <v>3</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="42">
+        <v>3</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C9" s="20">
+        <v>44956</v>
+      </c>
+      <c r="D9" s="21">
+        <v>44957</v>
+      </c>
+      <c r="E9" s="21">
+        <v>44958</v>
+      </c>
+      <c r="F9" s="21">
+        <v>44959</v>
+      </c>
+      <c r="G9" s="21">
+        <v>44960</v>
+      </c>
+      <c r="H9" s="21">
+        <v>44961</v>
+      </c>
+      <c r="I9" s="22">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="35">
+        <v>4</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="42">
+        <v>4</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C11" s="20">
+        <v>44963</v>
+      </c>
+      <c r="D11" s="21">
+        <v>44964</v>
+      </c>
+      <c r="E11" s="21">
+        <v>44965</v>
+      </c>
+      <c r="F11" s="21">
+        <v>44966</v>
+      </c>
+      <c r="G11" s="21">
+        <v>44967</v>
+      </c>
+      <c r="H11" s="21">
+        <v>44968</v>
+      </c>
+      <c r="I11" s="22">
+        <v>44969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="37">
+        <v>5</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>583</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="43">
+        <v>5</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C13" s="26">
+        <v>44970</v>
+      </c>
+      <c r="D13" s="27">
+        <v>44971</v>
+      </c>
+      <c r="E13" s="27">
+        <v>44972</v>
+      </c>
+      <c r="F13" s="27">
+        <v>44973</v>
+      </c>
+      <c r="G13" s="27">
+        <v>44974</v>
+      </c>
+      <c r="H13" s="27">
+        <v>44975</v>
+      </c>
+      <c r="I13" s="28">
+        <v>44976</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="38">
+        <v>6</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="44">
+        <v>6</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C15" s="32">
+        <v>44977</v>
+      </c>
+      <c r="D15" s="33">
+        <v>44978</v>
+      </c>
+      <c r="E15" s="33">
+        <v>44979</v>
+      </c>
+      <c r="F15" s="33">
+        <v>44980</v>
+      </c>
+      <c r="G15" s="33">
+        <v>44981</v>
+      </c>
+      <c r="H15" s="33">
+        <v>44982</v>
+      </c>
+      <c r="I15" s="34">
+        <v>44983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="39">
+        <v>7</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="44">
+        <v>7</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C17" s="9">
+        <v>44984</v>
+      </c>
+      <c r="D17" s="10">
+        <v>44985</v>
+      </c>
+      <c r="E17" s="10">
+        <v>44986</v>
+      </c>
+      <c r="F17" s="10">
+        <v>44987</v>
+      </c>
+      <c r="G17" s="10">
+        <v>44988</v>
+      </c>
+      <c r="H17" s="10">
+        <v>44989</v>
+      </c>
+      <c r="I17" s="11">
+        <v>44990</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="39">
+        <v>8</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="44">
+        <v>8</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C19" s="9">
+        <v>44991</v>
+      </c>
+      <c r="D19" s="10">
+        <v>44992</v>
+      </c>
+      <c r="E19" s="10">
+        <v>44993</v>
+      </c>
+      <c r="F19" s="10">
+        <v>44994</v>
+      </c>
+      <c r="G19" s="10">
+        <v>44995</v>
+      </c>
+      <c r="H19" s="10">
+        <v>44996</v>
+      </c>
+      <c r="I19" s="11">
+        <v>44997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="39">
+        <v>9</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="44">
+        <v>9</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C21" s="9">
+        <v>44998</v>
+      </c>
+      <c r="D21" s="10">
+        <v>44999</v>
+      </c>
+      <c r="E21" s="10">
+        <v>45000</v>
+      </c>
+      <c r="F21" s="10">
+        <v>45001</v>
+      </c>
+      <c r="G21" s="10">
+        <v>45002</v>
+      </c>
+      <c r="H21" s="10">
+        <v>45003</v>
+      </c>
+      <c r="I21" s="11">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="39">
+        <v>10</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="44">
+        <v>10</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C23" s="9">
+        <v>45005</v>
+      </c>
+      <c r="D23" s="10">
+        <v>45006</v>
+      </c>
+      <c r="E23" s="10">
+        <v>45007</v>
+      </c>
+      <c r="F23" s="10">
+        <v>45008</v>
+      </c>
+      <c r="G23" s="10">
+        <v>45009</v>
+      </c>
+      <c r="H23" s="10">
+        <v>45010</v>
+      </c>
+      <c r="I23" s="11">
+        <v>45011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="39">
+        <v>11</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="44">
+        <v>11</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C25" s="9">
+        <v>45012</v>
+      </c>
+      <c r="D25" s="10">
+        <v>45013</v>
+      </c>
+      <c r="E25" s="10">
+        <v>45014</v>
+      </c>
+      <c r="F25" s="10">
+        <v>45015</v>
+      </c>
+      <c r="G25" s="10">
+        <v>45016</v>
+      </c>
+      <c r="H25" s="10">
+        <v>45017</v>
+      </c>
+      <c r="I25" s="11">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="39">
+        <v>12</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="44">
+        <v>12</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C27" s="9">
+        <v>45019</v>
+      </c>
+      <c r="D27" s="10">
+        <v>45020</v>
+      </c>
+      <c r="E27" s="10">
+        <v>45021</v>
+      </c>
+      <c r="F27" s="10">
+        <v>45022</v>
+      </c>
+      <c r="G27" s="10">
+        <v>45023</v>
+      </c>
+      <c r="H27" s="10">
+        <v>45024</v>
+      </c>
+      <c r="I27" s="11">
+        <v>45025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="39">
+        <v>13</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="44">
+        <v>13</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C29" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D29" s="10">
+        <v>45027</v>
+      </c>
+      <c r="E29" s="10">
+        <v>45028</v>
+      </c>
+      <c r="F29" s="10">
+        <v>45029</v>
+      </c>
+      <c r="G29" s="10">
+        <v>45030</v>
+      </c>
+      <c r="H29" s="10">
+        <v>45031</v>
+      </c>
+      <c r="I29" s="11">
+        <v>45032</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="39">
+        <v>14</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="44">
+        <v>14</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C31" s="9">
+        <v>45033</v>
+      </c>
+      <c r="D31" s="10">
+        <v>45034</v>
+      </c>
+      <c r="E31" s="10">
+        <v>45035</v>
+      </c>
+      <c r="F31" s="10">
+        <v>45036</v>
+      </c>
+      <c r="G31" s="10">
+        <v>45037</v>
+      </c>
+      <c r="H31" s="10">
+        <v>45038</v>
+      </c>
+      <c r="I31" s="11">
+        <v>45039</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="39">
+        <v>15</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="44">
+        <v>15</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C33" s="9">
+        <v>45040</v>
+      </c>
+      <c r="D33" s="10">
+        <v>45041</v>
+      </c>
+      <c r="E33" s="10">
+        <v>45042</v>
+      </c>
+      <c r="F33" s="10">
+        <v>45043</v>
+      </c>
+      <c r="G33" s="10">
+        <v>45044</v>
+      </c>
+      <c r="H33" s="10">
+        <v>45045</v>
+      </c>
+      <c r="I33" s="11">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="39">
+        <v>16</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="44">
+        <v>16</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C35" s="9">
+        <v>45047</v>
+      </c>
+      <c r="D35" s="10">
+        <v>45048</v>
+      </c>
+      <c r="E35" s="10">
+        <v>45049</v>
+      </c>
+      <c r="F35" s="10">
+        <v>45050</v>
+      </c>
+      <c r="G35" s="10">
+        <v>45051</v>
+      </c>
+      <c r="H35" s="10">
+        <v>45052</v>
+      </c>
+      <c r="I35" s="11">
+        <v>45053</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="39">
+        <v>17</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="44">
+        <v>17</v>
+      </c>
+      <c r="B37" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C37" s="9">
+        <v>45054</v>
+      </c>
+      <c r="D37" s="10">
+        <v>45055</v>
+      </c>
+      <c r="E37" s="10">
+        <v>45056</v>
+      </c>
+      <c r="F37" s="10">
+        <v>45057</v>
+      </c>
+      <c r="G37" s="10">
+        <v>45058</v>
+      </c>
+      <c r="H37" s="10">
+        <v>45059</v>
+      </c>
+      <c r="I37" s="11">
+        <v>45060</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="39">
+        <v>18</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="44">
+        <v>18</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C39" s="9">
+        <v>45061</v>
+      </c>
+      <c r="D39" s="10">
+        <v>45062</v>
+      </c>
+      <c r="E39" s="10">
+        <v>45063</v>
+      </c>
+      <c r="F39" s="10">
+        <v>45064</v>
+      </c>
+      <c r="G39" s="10">
+        <v>45065</v>
+      </c>
+      <c r="H39" s="10">
+        <v>45066</v>
+      </c>
+      <c r="I39" s="11">
+        <v>45067</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="39">
+        <v>19</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="44">
+        <v>19</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C41" s="9">
+        <v>45068</v>
+      </c>
+      <c r="D41" s="10">
+        <v>45069</v>
+      </c>
+      <c r="E41" s="10">
+        <v>45070</v>
+      </c>
+      <c r="F41" s="10">
+        <v>45071</v>
+      </c>
+      <c r="G41" s="10">
+        <v>45072</v>
+      </c>
+      <c r="H41" s="10">
+        <v>45073</v>
+      </c>
+      <c r="I41" s="11">
+        <v>45074</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="39">
+        <v>20</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="44">
+        <v>20</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C43" s="9">
+        <v>45075</v>
+      </c>
+      <c r="D43" s="10">
+        <v>45076</v>
+      </c>
+      <c r="E43" s="10">
+        <v>45077</v>
+      </c>
+      <c r="F43" s="10">
+        <v>45078</v>
+      </c>
+      <c r="G43" s="10">
+        <v>45079</v>
+      </c>
+      <c r="H43" s="10">
+        <v>45080</v>
+      </c>
+      <c r="I43" s="11">
+        <v>45081</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="39">
+        <v>21</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="44">
+        <v>21</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C45" s="9">
+        <v>45082</v>
+      </c>
+      <c r="D45" s="10">
+        <v>45083</v>
+      </c>
+      <c r="E45" s="10">
+        <v>45084</v>
+      </c>
+      <c r="F45" s="10">
+        <v>45085</v>
+      </c>
+      <c r="G45" s="10">
+        <v>45086</v>
+      </c>
+      <c r="H45" s="10">
+        <v>45087</v>
+      </c>
+      <c r="I45" s="11">
+        <v>45088</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="39">
+        <v>22</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="44">
+        <v>22</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C47" s="9">
+        <v>45089</v>
+      </c>
+      <c r="D47" s="10">
+        <v>45090</v>
+      </c>
+      <c r="E47" s="10">
+        <v>45091</v>
+      </c>
+      <c r="F47" s="10">
+        <v>45092</v>
+      </c>
+      <c r="G47" s="10">
+        <v>45093</v>
+      </c>
+      <c r="H47" s="10">
+        <v>45094</v>
+      </c>
+      <c r="I47" s="11">
+        <v>45095</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="39">
+        <v>23</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="44">
+        <v>23</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C49" s="9">
+        <v>45096</v>
+      </c>
+      <c r="D49" s="10">
+        <v>45097</v>
+      </c>
+      <c r="E49" s="10">
+        <v>45098</v>
+      </c>
+      <c r="F49" s="10">
+        <v>45099</v>
+      </c>
+      <c r="G49" s="10">
+        <v>45100</v>
+      </c>
+      <c r="H49" s="10">
+        <v>45101</v>
+      </c>
+      <c r="I49" s="11">
+        <v>45102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="39">
+        <v>24</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="44">
+        <v>24</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C51" s="9">
+        <v>45103</v>
+      </c>
+      <c r="D51" s="10">
+        <v>45104</v>
+      </c>
+      <c r="E51" s="10">
+        <v>45105</v>
+      </c>
+      <c r="F51" s="10">
+        <v>45106</v>
+      </c>
+      <c r="G51" s="10">
+        <v>45107</v>
+      </c>
+      <c r="H51" s="10">
+        <v>45108</v>
+      </c>
+      <c r="I51" s="11">
+        <v>45109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="39">
+        <v>25</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="44">
+        <v>25</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C53" s="9">
+        <v>45110</v>
+      </c>
+      <c r="D53" s="10">
+        <v>45111</v>
+      </c>
+      <c r="E53" s="10">
+        <v>45112</v>
+      </c>
+      <c r="F53" s="10">
+        <v>45113</v>
+      </c>
+      <c r="G53" s="10">
+        <v>45114</v>
+      </c>
+      <c r="H53" s="10">
+        <v>45115</v>
+      </c>
+      <c r="I53" s="11">
+        <v>45116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="39">
+        <v>26</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="44">
+        <v>26</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C55" s="9">
+        <v>45117</v>
+      </c>
+      <c r="D55" s="10">
+        <v>45118</v>
+      </c>
+      <c r="E55" s="10">
+        <v>45119</v>
+      </c>
+      <c r="F55" s="10">
+        <v>45120</v>
+      </c>
+      <c r="G55" s="10">
+        <v>45121</v>
+      </c>
+      <c r="H55" s="10">
+        <v>45122</v>
+      </c>
+      <c r="I55" s="11">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="39">
+        <v>27</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="44">
+        <v>27</v>
+      </c>
+      <c r="B57" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C57" s="9">
+        <v>45124</v>
+      </c>
+      <c r="D57" s="10">
+        <v>45125</v>
+      </c>
+      <c r="E57" s="10">
+        <v>45126</v>
+      </c>
+      <c r="F57" s="10">
+        <v>45127</v>
+      </c>
+      <c r="G57" s="10">
+        <v>45128</v>
+      </c>
+      <c r="H57" s="10">
+        <v>45129</v>
+      </c>
+      <c r="I57" s="11">
+        <v>45130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="39">
+        <v>28</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="44">
+        <v>28</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C59" s="9">
+        <v>45131</v>
+      </c>
+      <c r="D59" s="10">
+        <v>45132</v>
+      </c>
+      <c r="E59" s="10">
+        <v>45133</v>
+      </c>
+      <c r="F59" s="10">
+        <v>45134</v>
+      </c>
+      <c r="G59" s="10">
+        <v>45135</v>
+      </c>
+      <c r="H59" s="10">
+        <v>45136</v>
+      </c>
+      <c r="I59" s="11">
+        <v>45137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="39">
+        <v>29</v>
+      </c>
+      <c r="B60" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="44">
+        <v>29</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C61" s="9">
+        <v>45138</v>
+      </c>
+      <c r="D61" s="10">
+        <v>45139</v>
+      </c>
+      <c r="E61" s="10">
+        <v>45140</v>
+      </c>
+      <c r="F61" s="10">
+        <v>45141</v>
+      </c>
+      <c r="G61" s="10">
+        <v>45142</v>
+      </c>
+      <c r="H61" s="10">
+        <v>45143</v>
+      </c>
+      <c r="I61" s="11">
+        <v>45144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="39">
+        <v>30</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="44">
+        <v>30</v>
+      </c>
+      <c r="B63" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C63" s="9">
+        <v>45145</v>
+      </c>
+      <c r="D63" s="10">
+        <v>45146</v>
+      </c>
+      <c r="E63" s="10">
+        <v>45147</v>
+      </c>
+      <c r="F63" s="10">
+        <v>45148</v>
+      </c>
+      <c r="G63" s="10">
+        <v>45149</v>
+      </c>
+      <c r="H63" s="10">
+        <v>45150</v>
+      </c>
+      <c r="I63" s="11">
+        <v>45151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="39">
+        <v>31</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="44">
+        <v>31</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C65" s="9">
+        <v>45152</v>
+      </c>
+      <c r="D65" s="10">
+        <v>45153</v>
+      </c>
+      <c r="E65" s="10">
+        <v>45154</v>
+      </c>
+      <c r="F65" s="10">
+        <v>45155</v>
+      </c>
+      <c r="G65" s="10">
+        <v>45156</v>
+      </c>
+      <c r="H65" s="10">
+        <v>45157</v>
+      </c>
+      <c r="I65" s="11">
+        <v>45158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="39">
+        <v>32</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="44">
+        <v>32</v>
+      </c>
+      <c r="B67" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C67" s="9">
+        <v>45159</v>
+      </c>
+      <c r="D67" s="10">
+        <v>45160</v>
+      </c>
+      <c r="E67" s="10">
+        <v>45161</v>
+      </c>
+      <c r="F67" s="10">
+        <v>45162</v>
+      </c>
+      <c r="G67" s="10">
+        <v>45163</v>
+      </c>
+      <c r="H67" s="10">
+        <v>45164</v>
+      </c>
+      <c r="I67" s="11">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="39">
+        <v>33</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="44">
+        <v>33</v>
+      </c>
+      <c r="B69" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C69" s="9">
+        <v>45166</v>
+      </c>
+      <c r="D69" s="10">
+        <v>45167</v>
+      </c>
+      <c r="E69" s="10">
+        <v>45168</v>
+      </c>
+      <c r="F69" s="10">
+        <v>45169</v>
+      </c>
+      <c r="G69" s="10">
+        <v>45170</v>
+      </c>
+      <c r="H69" s="10">
+        <v>45171</v>
+      </c>
+      <c r="I69" s="11">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="39">
+        <v>34</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="44">
+        <v>34</v>
+      </c>
+      <c r="B71" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C71" s="9">
+        <v>45173</v>
+      </c>
+      <c r="D71" s="10">
+        <v>45174</v>
+      </c>
+      <c r="E71" s="10">
+        <v>45175</v>
+      </c>
+      <c r="F71" s="10">
+        <v>45176</v>
+      </c>
+      <c r="G71" s="10">
+        <v>45177</v>
+      </c>
+      <c r="H71" s="10">
+        <v>45178</v>
+      </c>
+      <c r="I71" s="11">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="39">
+        <v>35</v>
+      </c>
+      <c r="B72" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="44">
+        <v>35</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C73" s="9">
+        <v>45180</v>
+      </c>
+      <c r="D73" s="10">
+        <v>45181</v>
+      </c>
+      <c r="E73" s="10">
+        <v>45182</v>
+      </c>
+      <c r="F73" s="10">
+        <v>45183</v>
+      </c>
+      <c r="G73" s="10">
+        <v>45184</v>
+      </c>
+      <c r="H73" s="10">
+        <v>45185</v>
+      </c>
+      <c r="I73" s="11">
+        <v>45186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="39">
+        <v>36</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="44">
+        <v>36</v>
+      </c>
+      <c r="B75" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C75" s="9">
+        <v>45187</v>
+      </c>
+      <c r="D75" s="10">
+        <v>45188</v>
+      </c>
+      <c r="E75" s="10">
+        <v>45189</v>
+      </c>
+      <c r="F75" s="10">
+        <v>45190</v>
+      </c>
+      <c r="G75" s="10">
+        <v>45191</v>
+      </c>
+      <c r="H75" s="10">
+        <v>45192</v>
+      </c>
+      <c r="I75" s="11">
+        <v>45193</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="39">
+        <v>37</v>
+      </c>
+      <c r="B76" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="44">
+        <v>37</v>
+      </c>
+      <c r="B77" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C77" s="9">
+        <v>45194</v>
+      </c>
+      <c r="D77" s="10">
+        <v>45195</v>
+      </c>
+      <c r="E77" s="10">
+        <v>45196</v>
+      </c>
+      <c r="F77" s="10">
+        <v>45197</v>
+      </c>
+      <c r="G77" s="10">
+        <v>45198</v>
+      </c>
+      <c r="H77" s="10">
+        <v>45199</v>
+      </c>
+      <c r="I77" s="11">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="39">
+        <v>38</v>
+      </c>
+      <c r="B78" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="44">
+        <v>38</v>
+      </c>
+      <c r="B79" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C79" s="9">
+        <v>45201</v>
+      </c>
+      <c r="D79" s="10">
+        <v>45202</v>
+      </c>
+      <c r="E79" s="10">
+        <v>45203</v>
+      </c>
+      <c r="F79" s="10">
+        <v>45204</v>
+      </c>
+      <c r="G79" s="10">
+        <v>45205</v>
+      </c>
+      <c r="H79" s="10">
+        <v>45206</v>
+      </c>
+      <c r="I79" s="11">
+        <v>45207</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="39">
+        <v>39</v>
+      </c>
+      <c r="B80" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="44">
+        <v>39</v>
+      </c>
+      <c r="B81" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C81" s="9">
+        <v>45208</v>
+      </c>
+      <c r="D81" s="10">
+        <v>45209</v>
+      </c>
+      <c r="E81" s="10">
+        <v>45210</v>
+      </c>
+      <c r="F81" s="10">
+        <v>45211</v>
+      </c>
+      <c r="G81" s="10">
+        <v>45212</v>
+      </c>
+      <c r="H81" s="10">
+        <v>45213</v>
+      </c>
+      <c r="I81" s="11">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="39">
+        <v>40</v>
+      </c>
+      <c r="B82" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="44">
+        <v>40</v>
+      </c>
+      <c r="B83" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C83" s="9">
+        <v>45215</v>
+      </c>
+      <c r="D83" s="10">
+        <v>45216</v>
+      </c>
+      <c r="E83" s="10">
+        <v>45217</v>
+      </c>
+      <c r="F83" s="10">
+        <v>45218</v>
+      </c>
+      <c r="G83" s="10">
+        <v>45219</v>
+      </c>
+      <c r="H83" s="10">
+        <v>45220</v>
+      </c>
+      <c r="I83" s="11">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="39">
+        <v>41</v>
+      </c>
+      <c r="B84" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="44">
+        <v>41</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C85" s="9">
+        <v>45222</v>
+      </c>
+      <c r="D85" s="10">
+        <v>45223</v>
+      </c>
+      <c r="E85" s="10">
+        <v>45224</v>
+      </c>
+      <c r="F85" s="10">
+        <v>45225</v>
+      </c>
+      <c r="G85" s="10">
+        <v>45226</v>
+      </c>
+      <c r="H85" s="10">
+        <v>45227</v>
+      </c>
+      <c r="I85" s="11">
+        <v>45228</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="39">
+        <v>42</v>
+      </c>
+      <c r="B86" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="44">
+        <v>42</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C87" s="9">
+        <v>45229</v>
+      </c>
+      <c r="D87" s="10">
+        <v>45230</v>
+      </c>
+      <c r="E87" s="10">
+        <v>45231</v>
+      </c>
+      <c r="F87" s="10">
+        <v>45232</v>
+      </c>
+      <c r="G87" s="10">
+        <v>45233</v>
+      </c>
+      <c r="H87" s="10">
+        <v>45234</v>
+      </c>
+      <c r="I87" s="11">
+        <v>45235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="39">
+        <v>43</v>
+      </c>
+      <c r="B88" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="44">
+        <v>43</v>
+      </c>
+      <c r="B89" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C89" s="9">
+        <v>45236</v>
+      </c>
+      <c r="D89" s="10">
+        <v>45237</v>
+      </c>
+      <c r="E89" s="10">
+        <v>45238</v>
+      </c>
+      <c r="F89" s="10">
+        <v>45239</v>
+      </c>
+      <c r="G89" s="10">
+        <v>45240</v>
+      </c>
+      <c r="H89" s="10">
+        <v>45241</v>
+      </c>
+      <c r="I89" s="11">
+        <v>45242</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="39">
+        <v>44</v>
+      </c>
+      <c r="B90" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="44">
+        <v>44</v>
+      </c>
+      <c r="B91" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C91" s="9">
+        <v>45243</v>
+      </c>
+      <c r="D91" s="10">
+        <v>45244</v>
+      </c>
+      <c r="E91" s="10">
+        <v>45245</v>
+      </c>
+      <c r="F91" s="10">
+        <v>45246</v>
+      </c>
+      <c r="G91" s="10">
+        <v>45247</v>
+      </c>
+      <c r="H91" s="10">
+        <v>45248</v>
+      </c>
+      <c r="I91" s="11">
+        <v>45249</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="39">
+        <v>45</v>
+      </c>
+      <c r="B92" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="F92" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="44">
+        <v>45</v>
+      </c>
+      <c r="B93" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C93" s="9">
+        <v>45250</v>
+      </c>
+      <c r="D93" s="10">
+        <v>45251</v>
+      </c>
+      <c r="E93" s="10">
+        <v>45252</v>
+      </c>
+      <c r="F93" s="10">
+        <v>45253</v>
+      </c>
+      <c r="G93" s="10">
+        <v>45254</v>
+      </c>
+      <c r="H93" s="10">
+        <v>45255</v>
+      </c>
+      <c r="I93" s="11">
+        <v>45256</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="39">
+        <v>46</v>
+      </c>
+      <c r="B94" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="H94" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="44">
+        <v>46</v>
+      </c>
+      <c r="B95" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C95" s="9">
+        <v>45257</v>
+      </c>
+      <c r="D95" s="10">
+        <v>45258</v>
+      </c>
+      <c r="E95" s="10">
+        <v>45259</v>
+      </c>
+      <c r="F95" s="10">
+        <v>45260</v>
+      </c>
+      <c r="G95" s="10">
+        <v>45261</v>
+      </c>
+      <c r="H95" s="10">
+        <v>45262</v>
+      </c>
+      <c r="I95" s="11">
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="39">
+        <v>47</v>
+      </c>
+      <c r="B96" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="I96" s="6" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="44">
+        <v>47</v>
+      </c>
+      <c r="B97" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C97" s="9">
+        <v>45264</v>
+      </c>
+      <c r="D97" s="10">
+        <v>45265</v>
+      </c>
+      <c r="E97" s="10">
+        <v>45266</v>
+      </c>
+      <c r="F97" s="10">
+        <v>45267</v>
+      </c>
+      <c r="G97" s="10">
+        <v>45268</v>
+      </c>
+      <c r="H97" s="10">
+        <v>45269</v>
+      </c>
+      <c r="I97" s="11">
+        <v>45270</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="39">
+        <v>48</v>
+      </c>
+      <c r="B98" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="I98" s="6" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="44">
+        <v>48</v>
+      </c>
+      <c r="B99" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C99" s="9">
+        <v>45271</v>
+      </c>
+      <c r="D99" s="10">
+        <v>45272</v>
+      </c>
+      <c r="E99" s="10">
+        <v>45273</v>
+      </c>
+      <c r="F99" s="10">
+        <v>45274</v>
+      </c>
+      <c r="G99" s="10">
+        <v>45275</v>
+      </c>
+      <c r="H99" s="10">
+        <v>45276</v>
+      </c>
+      <c r="I99" s="11">
+        <v>45277</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="39">
+        <v>49</v>
+      </c>
+      <c r="B100" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="F100" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="H100" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="I100" s="6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="44">
+        <v>49</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C101" s="9">
+        <v>45278</v>
+      </c>
+      <c r="D101" s="10">
+        <v>45279</v>
+      </c>
+      <c r="E101" s="10">
+        <v>45280</v>
+      </c>
+      <c r="F101" s="10">
+        <v>45281</v>
+      </c>
+      <c r="G101" s="10">
+        <v>45282</v>
+      </c>
+      <c r="H101" s="10">
+        <v>45283</v>
+      </c>
+      <c r="I101" s="11">
+        <v>45284</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="39">
+        <v>50</v>
+      </c>
+      <c r="B102" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="G102" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="H102" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="I102" s="6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="44">
+        <v>50</v>
+      </c>
+      <c r="B103" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C103" s="9">
+        <v>45285</v>
+      </c>
+      <c r="D103" s="10">
+        <v>45286</v>
+      </c>
+      <c r="E103" s="10">
+        <v>45287</v>
+      </c>
+      <c r="F103" s="10">
+        <v>45288</v>
+      </c>
+      <c r="G103" s="10">
+        <v>45289</v>
+      </c>
+      <c r="H103" s="10">
+        <v>45290</v>
+      </c>
+      <c r="I103" s="11">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="39">
+        <v>51</v>
+      </c>
+      <c r="B104" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="F104" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="44">
+        <v>51</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C105" s="9">
+        <v>45292</v>
+      </c>
+      <c r="D105" s="10">
+        <v>45293</v>
+      </c>
+      <c r="E105" s="10">
+        <v>45294</v>
+      </c>
+      <c r="F105" s="10">
+        <v>45295</v>
+      </c>
+      <c r="G105" s="10">
+        <v>45296</v>
+      </c>
+      <c r="H105" s="10">
+        <v>45297</v>
+      </c>
+      <c r="I105" s="11">
+        <v>45298</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="39">
+        <v>52</v>
+      </c>
+      <c r="B106" s="35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>578</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="I106" s="6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="44">
+        <v>52</v>
+      </c>
+      <c r="B107" s="36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C107" s="12">
+        <v>45299</v>
+      </c>
+      <c r="D107" s="13">
+        <v>45300</v>
+      </c>
+      <c r="E107" s="13">
+        <v>45301</v>
+      </c>
+      <c r="F107" s="13">
+        <v>45302</v>
+      </c>
+      <c r="G107" s="13">
+        <v>45303</v>
+      </c>
+      <c r="H107" s="13">
+        <v>45304</v>
+      </c>
+      <c r="I107" s="14">
+        <v>45305</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:I107"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja5"/>
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>589</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>44970</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44971</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44972</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44973</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44974</v>
+      </c>
+      <c r="F3" s="3">
+        <v>44975</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44976</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>44977</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44978</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44979</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44980</v>
+      </c>
+      <c r="E4" s="3">
+        <v>44981</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44982</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44983</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>44984</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44985</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44986</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44987</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44988</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44989</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44990</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>44991</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44992</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44993</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44994</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44995</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44996</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>44998</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44999</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45002</v>
+      </c>
+      <c r="F7" s="3">
+        <v>45003</v>
+      </c>
+      <c r="G7" s="3">
+        <v>45004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>45005</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45006</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45007</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45008</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45009</v>
+      </c>
+      <c r="F8" s="3">
+        <v>45010</v>
+      </c>
+      <c r="G8" s="3">
+        <v>45011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>45012</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45013</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45014</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45015</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45016</v>
+      </c>
+      <c r="F9" s="3">
+        <v>45017</v>
+      </c>
+      <c r="G9" s="3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>45019</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45020</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45021</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45022</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45023</v>
+      </c>
+      <c r="F10" s="3">
+        <v>45024</v>
+      </c>
+      <c r="G10" s="3">
+        <v>45025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>45026</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45027</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45028</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45029</v>
+      </c>
+      <c r="E11" s="3">
+        <v>45030</v>
+      </c>
+      <c r="F11" s="3">
+        <v>45031</v>
+      </c>
+      <c r="G11" s="3">
+        <v>45032</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>45033</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45034</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45035</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45036</v>
+      </c>
+      <c r="E12" s="3">
+        <v>45037</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45038</v>
+      </c>
+      <c r="G12" s="3">
+        <v>45039</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>45040</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45041</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45042</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45043</v>
+      </c>
+      <c r="E13" s="3">
+        <v>45044</v>
+      </c>
+      <c r="F13" s="3">
+        <v>45045</v>
+      </c>
+      <c r="G13" s="3">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>45047</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45048</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45049</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45050</v>
+      </c>
+      <c r="E14" s="3">
+        <v>45051</v>
+      </c>
+      <c r="F14" s="3">
+        <v>45052</v>
+      </c>
+      <c r="G14" s="3">
+        <v>45053</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>45054</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45055</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45056</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45057</v>
+      </c>
+      <c r="E15" s="3">
+        <v>45058</v>
+      </c>
+      <c r="F15" s="3">
+        <v>45059</v>
+      </c>
+      <c r="G15" s="3">
+        <v>45060</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>45061</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45062</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45063</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45064</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45065</v>
+      </c>
+      <c r="F16" s="3">
+        <v>45066</v>
+      </c>
+      <c r="G16" s="3">
+        <v>45067</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>45068</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45069</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45070</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45071</v>
+      </c>
+      <c r="E17" s="3">
+        <v>45072</v>
+      </c>
+      <c r="F17" s="3">
+        <v>45073</v>
+      </c>
+      <c r="G17" s="3">
+        <v>45074</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>45075</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45076</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45077</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45078</v>
+      </c>
+      <c r="E18" s="3">
+        <v>45079</v>
+      </c>
+      <c r="F18" s="3">
+        <v>45080</v>
+      </c>
+      <c r="G18" s="3">
+        <v>45081</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>45082</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45083</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45084</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45085</v>
+      </c>
+      <c r="E19" s="3">
+        <v>45086</v>
+      </c>
+      <c r="F19" s="3">
+        <v>45087</v>
+      </c>
+      <c r="G19" s="3">
+        <v>45088</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>45089</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45090</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45091</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45092</v>
+      </c>
+      <c r="E20" s="3">
+        <v>45093</v>
+      </c>
+      <c r="F20" s="3">
+        <v>45094</v>
+      </c>
+      <c r="G20" s="3">
+        <v>45095</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>45096</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45097</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45098</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45099</v>
+      </c>
+      <c r="E21" s="3">
+        <v>45100</v>
+      </c>
+      <c r="F21" s="3">
+        <v>45101</v>
+      </c>
+      <c r="G21" s="3">
+        <v>45102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>45103</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45104</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45105</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45106</v>
+      </c>
+      <c r="E22" s="3">
+        <v>45107</v>
+      </c>
+      <c r="F22" s="3">
+        <v>45108</v>
+      </c>
+      <c r="G22" s="3">
+        <v>45109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>45110</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45111</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45112</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45113</v>
+      </c>
+      <c r="E23" s="3">
+        <v>45114</v>
+      </c>
+      <c r="F23" s="3">
+        <v>45115</v>
+      </c>
+      <c r="G23" s="3">
+        <v>45116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>45117</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45118</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45119</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45120</v>
+      </c>
+      <c r="E24" s="3">
+        <v>45121</v>
+      </c>
+      <c r="F24" s="3">
+        <v>45122</v>
+      </c>
+      <c r="G24" s="3">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>45124</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45125</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45126</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45127</v>
+      </c>
+      <c r="E25" s="3">
+        <v>45128</v>
+      </c>
+      <c r="F25" s="3">
+        <v>45129</v>
+      </c>
+      <c r="G25" s="3">
+        <v>45130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>45131</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45132</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45133</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45134</v>
+      </c>
+      <c r="E26" s="3">
+        <v>45135</v>
+      </c>
+      <c r="F26" s="3">
+        <v>45136</v>
+      </c>
+      <c r="G26" s="3">
+        <v>45137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>45138</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45139</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45140</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45141</v>
+      </c>
+      <c r="E27" s="3">
+        <v>45142</v>
+      </c>
+      <c r="F27" s="3">
+        <v>45143</v>
+      </c>
+      <c r="G27" s="3">
+        <v>45144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>45145</v>
+      </c>
+      <c r="B28" s="3">
+        <v>45146</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45147</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45148</v>
+      </c>
+      <c r="E28" s="3">
+        <v>45149</v>
+      </c>
+      <c r="F28" s="3">
+        <v>45150</v>
+      </c>
+      <c r="G28" s="3">
+        <v>45151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>45152</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45153</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45154</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45155</v>
+      </c>
+      <c r="E29" s="3">
+        <v>45156</v>
+      </c>
+      <c r="F29" s="3">
+        <v>45157</v>
+      </c>
+      <c r="G29" s="3">
+        <v>45158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>45159</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45160</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45161</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45162</v>
+      </c>
+      <c r="E30" s="3">
+        <v>45163</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45164</v>
+      </c>
+      <c r="G30" s="3">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>45166</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45167</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45168</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45169</v>
+      </c>
+      <c r="E31" s="3">
+        <v>45170</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45171</v>
+      </c>
+      <c r="G31" s="3">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>45173</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45174</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45175</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45176</v>
+      </c>
+      <c r="E32" s="3">
+        <v>45177</v>
+      </c>
+      <c r="F32" s="3">
+        <v>45178</v>
+      </c>
+      <c r="G32" s="3">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>45180</v>
+      </c>
+      <c r="B33" s="3">
+        <v>45181</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45182</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45183</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45184</v>
+      </c>
+      <c r="F33" s="3">
+        <v>45185</v>
+      </c>
+      <c r="G33" s="3">
+        <v>45186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>45187</v>
+      </c>
+      <c r="B34" s="3">
+        <v>45188</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45189</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45190</v>
+      </c>
+      <c r="E34" s="3">
+        <v>45191</v>
+      </c>
+      <c r="F34" s="3">
+        <v>45192</v>
+      </c>
+      <c r="G34" s="3">
+        <v>45193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>45194</v>
+      </c>
+      <c r="B35" s="3">
+        <v>45195</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45196</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45197</v>
+      </c>
+      <c r="E35" s="3">
+        <v>45198</v>
+      </c>
+      <c r="F35" s="3">
+        <v>45199</v>
+      </c>
+      <c r="G35" s="3">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>45201</v>
+      </c>
+      <c r="B36" s="3">
+        <v>45202</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45203</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45204</v>
+      </c>
+      <c r="E36" s="3">
+        <v>45205</v>
+      </c>
+      <c r="F36" s="3">
+        <v>45206</v>
+      </c>
+      <c r="G36" s="3">
+        <v>45207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>45208</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45209</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45210</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45211</v>
+      </c>
+      <c r="E37" s="3">
+        <v>45212</v>
+      </c>
+      <c r="F37" s="3">
+        <v>45213</v>
+      </c>
+      <c r="G37" s="3">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>45215</v>
+      </c>
+      <c r="B38" s="3">
+        <v>45216</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45217</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45218</v>
+      </c>
+      <c r="E38" s="3">
+        <v>45219</v>
+      </c>
+      <c r="F38" s="3">
+        <v>45220</v>
+      </c>
+      <c r="G38" s="3">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>45222</v>
+      </c>
+      <c r="B39" s="3">
+        <v>45223</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45224</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45225</v>
+      </c>
+      <c r="E39" s="3">
+        <v>45226</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45227</v>
+      </c>
+      <c r="G39" s="3">
+        <v>45228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>45229</v>
+      </c>
+      <c r="B40" s="3">
+        <v>45230</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45231</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45232</v>
+      </c>
+      <c r="E40" s="3">
+        <v>45233</v>
+      </c>
+      <c r="F40" s="3">
+        <v>45234</v>
+      </c>
+      <c r="G40" s="3">
+        <v>45235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>45236</v>
+      </c>
+      <c r="B41" s="3">
+        <v>45237</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45238</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45239</v>
+      </c>
+      <c r="E41" s="3">
+        <v>45240</v>
+      </c>
+      <c r="F41" s="3">
+        <v>45241</v>
+      </c>
+      <c r="G41" s="3">
+        <v>45242</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>45243</v>
+      </c>
+      <c r="B42" s="3">
+        <v>45244</v>
+      </c>
+      <c r="C42" s="3">
+        <v>45245</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45246</v>
+      </c>
+      <c r="E42" s="3">
+        <v>45247</v>
+      </c>
+      <c r="F42" s="3">
+        <v>45248</v>
+      </c>
+      <c r="G42" s="3">
+        <v>45249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>45250</v>
+      </c>
+      <c r="B43" s="3">
+        <v>45251</v>
+      </c>
+      <c r="C43" s="3">
+        <v>45252</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45253</v>
+      </c>
+      <c r="E43" s="3">
+        <v>45254</v>
+      </c>
+      <c r="F43" s="3">
+        <v>45255</v>
+      </c>
+      <c r="G43" s="3">
+        <v>45256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>45257</v>
+      </c>
+      <c r="B44" s="3">
+        <v>45258</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45259</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45260</v>
+      </c>
+      <c r="E44" s="3">
+        <v>45261</v>
+      </c>
+      <c r="F44" s="3">
+        <v>45262</v>
+      </c>
+      <c r="G44" s="3">
+        <v>45263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>45264</v>
+      </c>
+      <c r="B45" s="3">
+        <v>45265</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45266</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45267</v>
+      </c>
+      <c r="E45" s="3">
+        <v>45268</v>
+      </c>
+      <c r="F45" s="3">
+        <v>45269</v>
+      </c>
+      <c r="G45" s="3">
+        <v>45270</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>45271</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45272</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45273</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45274</v>
+      </c>
+      <c r="E46" s="3">
+        <v>45275</v>
+      </c>
+      <c r="F46" s="3">
+        <v>45276</v>
+      </c>
+      <c r="G46" s="3">
+        <v>45277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>45278</v>
+      </c>
+      <c r="B47" s="3">
+        <v>45279</v>
+      </c>
+      <c r="C47" s="3">
+        <v>45280</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45281</v>
+      </c>
+      <c r="E47" s="3">
+        <v>45282</v>
+      </c>
+      <c r="F47" s="3">
+        <v>45283</v>
+      </c>
+      <c r="G47" s="3">
+        <v>45284</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>45285</v>
+      </c>
+      <c r="B48" s="3">
+        <v>45286</v>
+      </c>
+      <c r="C48" s="3">
+        <v>45287</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45288</v>
+      </c>
+      <c r="E48" s="3">
+        <v>45289</v>
+      </c>
+      <c r="F48" s="3">
+        <v>45290</v>
+      </c>
+      <c r="G48" s="3">
+        <v>45291</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>